<commit_message>
introduce Views.adl and make AST.adl  compilable.
</commit_message>
<xml_diff>
--- a/AmpersandData/FormalAmpersand/Views.xlsx
+++ b/AmpersandData/FormalAmpersand/Views.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="29">
   <si>
     <t>[Concept]</t>
   </si>
@@ -39,12 +39,6 @@
     <t>repr</t>
   </si>
   <si>
-    <t>Term</t>
-  </si>
-  <si>
-    <t>Composition</t>
-  </si>
-  <si>
     <t>pop</t>
   </si>
   <si>
@@ -57,12 +51,6 @@
     <t>[View]</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
     <t>concept</t>
   </si>
   <si>
@@ -75,7 +63,46 @@
     <t>drie</t>
   </si>
   <si>
-    <t>Term,Composition</t>
+    <t>Fruit</t>
+  </si>
+  <si>
+    <t>Citrus</t>
+  </si>
+  <si>
+    <t>Lime</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Limo</t>
+  </si>
+  <si>
+    <t>vier</t>
+  </si>
+  <si>
+    <t>zes</t>
+  </si>
+  <si>
+    <t>Spanje</t>
+  </si>
+  <si>
+    <t>Andalusie</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Mars</t>
+  </si>
+  <si>
+    <t>Europa</t>
+  </si>
+  <si>
+    <t>Identifier</t>
+  </si>
+  <si>
+    <t>Representation</t>
   </si>
 </sst>
 </file>
@@ -415,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,48 +458,148 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="1" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
-        <v>8</v>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -482,7 +609,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -505,27 +632,71 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -535,44 +706,68 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD7"/>
+      <selection activeCell="E5" sqref="E5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>